<commit_message>
Second commit for practice
</commit_message>
<xml_diff>
--- a/cucumberjvm-selenium-pageobject/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/cucumberjvm-selenium-pageobject/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="19845" windowHeight="4665" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="4350" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -65,12 +65,6 @@
     <t>FRA</t>
   </si>
   <si>
-    <t>09092018</t>
-  </si>
-  <si>
-    <t>19092018</t>
-  </si>
-  <si>
     <t>ghgf</t>
   </si>
   <si>
@@ -86,10 +80,16 @@
     <t>Gopal Varma</t>
   </si>
   <si>
-    <t>a68er12</t>
-  </si>
-  <si>
     <t>ber</t>
+  </si>
+  <si>
+    <t>Serv014ice</t>
+  </si>
+  <si>
+    <t>03062019</t>
+  </si>
+  <si>
+    <t>10062019</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,7 +358,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,10 +622,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>179001</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>11</v>
@@ -648,22 +648,22 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="K2" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>